<commit_message>
Load parameters from dataframe for Depression
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression.xlsx
+++ b/resources/ResourceFile_Depression.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Phillips\PycharmProjects\TLOmodel\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63BAB66-3E18-6B4F-BB8B-D16BEBD132FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="2620" windowWidth="22920" windowHeight="13680" activeTab="1"/>
+    <workbookView xWindow="33960" yWindow="-22580" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="575">
   <si>
     <t>Name:</t>
   </si>
@@ -1781,9 +1782,6 @@
     <t>rr_resol_depr_on_antidepr</t>
   </si>
   <si>
-    <t>rate_init_antidep</t>
-  </si>
-  <si>
     <t>prob_3m_suicide_depr_m</t>
   </si>
   <si>
@@ -1791,12 +1789,21 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>init_rp_ever_depr_not_current</t>
+  </si>
+  <si>
+    <t>daly_wt_severe_episode_major_depressive_disorder</t>
+  </si>
+  <si>
+    <t>daly_wt_moderate_episode_major_depressive_disorder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2119,7 +2126,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5062AFF-693C-6A42-A173-3AAA30FCCCE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2186,7 +2193,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B8C12E02-291F-F142-BE0B-B89AA58E6F86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2267,7 +2274,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37"/>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2305,7 +2318,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2348,7 +2367,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2403,7 +2428,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2458,7 +2489,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2513,7 +2550,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2568,7 +2611,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2623,7 +2672,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2678,7 +2733,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3017,20 +3078,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="90.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3038,25 +3099,25 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
@@ -3064,10 +3125,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
@@ -3075,34 +3136,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3110,7 +3171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
@@ -3118,7 +3179,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
@@ -3126,19 +3187,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
@@ -3146,19 +3207,19 @@
         <v>43346</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
       <c r="C26" s="8"/>
     </row>
@@ -3169,21 +3230,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.9140625" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>109</v>
       </c>
@@ -3202,7 +3263,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -3223,7 +3284,7 @@
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -3237,7 +3298,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3251,7 +3312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -3271,14 +3332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
@@ -3287,7 +3348,7 @@
     <col min="5" max="5" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>160</v>
       </c>
@@ -3301,13 +3362,13 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="C3" s="27" t="s">
         <v>532</v>
@@ -3316,7 +3377,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>186</v>
       </c>
@@ -3327,7 +3388,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>179</v>
       </c>
@@ -3338,7 +3399,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>180</v>
       </c>
@@ -3349,7 +3410,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>181</v>
       </c>
@@ -3360,7 +3421,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>182</v>
       </c>
@@ -3371,7 +3432,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>183</v>
       </c>
@@ -3382,7 +3443,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>184</v>
       </c>
@@ -3393,7 +3454,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>185</v>
       </c>
@@ -3404,7 +3465,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>158</v>
       </c>
@@ -3416,7 +3477,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>65</v>
       </c>
@@ -3427,7 +3488,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>66</v>
       </c>
@@ -3438,7 +3499,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>67</v>
       </c>
@@ -3449,7 +3510,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>68</v>
       </c>
@@ -3460,7 +3521,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>69</v>
       </c>
@@ -3471,7 +3532,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>187</v>
       </c>
@@ -3482,7 +3543,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>188</v>
       </c>
@@ -3499,16 +3560,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B2:O598"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -3516,68 +3577,68 @@
         <v>527</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>210</v>
       </c>
@@ -3585,2052 +3646,2052 @@
         <v>528</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C154" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D233" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D234" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D235" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D236" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D237" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D238" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D239" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B282" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B284" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B285" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B287" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B288" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B289" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B291" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B292" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B293" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B295" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B296" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B297" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B298" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B299" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B301" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="302" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B302" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="303" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B303" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="306" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B306" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="307" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B307" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B308" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B309" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B310" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B312" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B313" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B314" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B316" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B322" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="324" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B324" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="325" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B325" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="326" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B326" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B328" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B329" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B330" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B332" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B333" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B334" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B336" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="337" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B337" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="338" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B338" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="340" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B340" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="343" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B343" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="345" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B345" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="347" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C347" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="349" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C349" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="350" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C350" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="351" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C351" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="352" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C352" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="353" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="353" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C353" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="354" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="354" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D354" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="355" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="355" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C355" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="357" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="357" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C357" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="360" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="360" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C360" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="362" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="362" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C362" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="365" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="365" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C365" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="367" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="367" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C367" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="368" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="368" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C368" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C369" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C372" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C374" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C375" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C377" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C379" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B381" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B384" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B386" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B387" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="388" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B388" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="389" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B389" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="393" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B393" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="395" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B395" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="397" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C397" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="398" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C398" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="399" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C399" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="400" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C400" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="401" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="401" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C401" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="402" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="402" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C402" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="403" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="403" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C403" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="404" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="404" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C404" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="405" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="405" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C405" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="406" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="406" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C406" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="407" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="407" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C407" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="408" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="408" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C408" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="409" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="409" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D409" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="410" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="410" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D410" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="411" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="411" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D411" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="412" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="412" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D412" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="413" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="413" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D413" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="414" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="414" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D414" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="415" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="415" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D415" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="416" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="416" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C416" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="418" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B418" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="421" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B421" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="423" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B423" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="424" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B424" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="425" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B425" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="428" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B428" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="430" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B430" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="431" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B431" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="432" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B432" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="433" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="433" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B433" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="434" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B434" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="435" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B435" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="438" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B438" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="440" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="440" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B440" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="441" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C441" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="442" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="442" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C442" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="443" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="443" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C443" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="444" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C444" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="445" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C445" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="446" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C446" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="447" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B447" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="449" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B449" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="453" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B453" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="455" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B455" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="456" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B456" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="459" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B459" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="461" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B461" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="462" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B462" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="465" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="465" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B465" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="467" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="467" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B467" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="468" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="468" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B468" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="469" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="469" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B469" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="474" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="474" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B474" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="475" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="475" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C475" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="476" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="476" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D476" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="477" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="477" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D477" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="478" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="478" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D478" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="479" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="479" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D479" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="480" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="480" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D480" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D481" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D482" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D483" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D484" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D485" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D486" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D487" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D488" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D489" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D490" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D491" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D492" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D493" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D494" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D495" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D496" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="497" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="497" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C497" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="499" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="499" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C499" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="500" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="500" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D500" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="501" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="501" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D501" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="502" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="502" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D502" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="503" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="503" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D503" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="504" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="504" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D504" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="505" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="505" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D505" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="506" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="506" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D506" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="507" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="507" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D507" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="508" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="508" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D508" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="509" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="509" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D509" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="510" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="510" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D510" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="511" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="511" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D511" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="512" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="512" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D512" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="513" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="513" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D513" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="514" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="514" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D514" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="515" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="515" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D515" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="516" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="516" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D516" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="517" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="517" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D517" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="518" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="518" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D518" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="519" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="519" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D519" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="520" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="520" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D520" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="521" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="521" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C521" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="523" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="523" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B523" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="524" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="524" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B524" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="525" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="525" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B525" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="527" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="527" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B527" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="528" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="528" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B528" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="529" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B529" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B531" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="532" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B532" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="534" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B534" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="535" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B535" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="537" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B537" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="539" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B539" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="541" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B541" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="542" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B542" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="543" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B543" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="548" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B548" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="549" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B549" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="552" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="552" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B552" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="553" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="553" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B553" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="554" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="554" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B554" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="555" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="555" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B555" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="556" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="556" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B556" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="557" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="557" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B557" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="558" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="558" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B558" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="560" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="560" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B560" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="561" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="561" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B561" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="562" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="562" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B562" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="563" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="563" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B563" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="565" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="565" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B565" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="566" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B566" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="567" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="567" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B567" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="568" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="568" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B568" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="570" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="570" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B570" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="571" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="571" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B571" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="572" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="572" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B572" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="573" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="573" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B573" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="574" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="574" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B574" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="575" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="575" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B575" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="576" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="576" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B576" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="577" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B577" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="579" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B579" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="580" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B580" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="582" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B582" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="583" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B583" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="585" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B585" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="586" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B586" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="587" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B587" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="589" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B589" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="591" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B591" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B592" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B594" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B596" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B598" t="s">
         <v>488</v>
       </c>
@@ -5642,20 +5703,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.08203125" customWidth="1"/>
-    <col min="2" max="2" width="24.08203125" customWidth="1"/>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>545</v>
       </c>
@@ -5663,7 +5724,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>546</v>
       </c>
@@ -5671,7 +5732,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>547</v>
       </c>
@@ -5679,7 +5740,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>548</v>
       </c>
@@ -5687,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>549</v>
       </c>
@@ -5698,7 +5759,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>550</v>
       </c>
@@ -5706,7 +5767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5714,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>552</v>
       </c>
@@ -5722,7 +5783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>553</v>
       </c>
@@ -5730,7 +5791,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>554</v>
       </c>
@@ -5738,7 +5799,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>555</v>
       </c>
@@ -5746,7 +5807,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>556</v>
       </c>
@@ -5754,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>557</v>
       </c>
@@ -5762,7 +5823,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>558</v>
       </c>
@@ -5770,7 +5831,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>559</v>
       </c>
@@ -5778,7 +5839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>560</v>
       </c>
@@ -5786,7 +5847,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>561</v>
       </c>
@@ -5797,7 +5858,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>562</v>
       </c>
@@ -5805,7 +5866,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -5813,7 +5874,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>563</v>
       </c>
@@ -5821,7 +5882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>564</v>
       </c>
@@ -5829,10 +5890,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>565</v>
       </c>
@@ -5840,7 +5901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>566</v>
       </c>
@@ -5848,7 +5909,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>567</v>
       </c>
@@ -5856,7 +5917,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>568</v>
       </c>
@@ -5864,15 +5925,15 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>569</v>
+        <v>57</v>
       </c>
       <c r="B26">
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -5880,7 +5941,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -5888,15 +5949,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B29">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>536</v>
       </c>
@@ -5904,12 +5965,36 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B31">
         <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>572</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>573</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>574</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5919,27 +6004,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A26:E76"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.08203125" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="95.9140625" customWidth="1"/>
+    <col min="4" max="4" width="95.83203125" customWidth="1"/>
     <col min="5" max="5" width="148.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>490</v>
       </c>
@@ -5950,7 +6035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -5961,7 +6046,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -5969,7 +6054,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -5980,7 +6065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -5991,7 +6076,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -5999,7 +6084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>53</v>
       </c>
@@ -6013,7 +6098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -6027,7 +6112,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>38</v>
       </c>
@@ -6041,7 +6126,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -6055,7 +6140,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -6069,7 +6154,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>44</v>
       </c>
@@ -6083,7 +6168,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>46</v>
       </c>
@@ -6097,7 +6182,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>48</v>
       </c>
@@ -6111,7 +6196,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -6125,7 +6210,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -6139,7 +6224,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>57</v>
       </c>
@@ -6153,7 +6238,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>59</v>
       </c>
@@ -6167,7 +6252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>61</v>
       </c>
@@ -6181,7 +6266,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>63</v>
       </c>
@@ -6195,7 +6280,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>65</v>
       </c>
@@ -6209,7 +6294,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>66</v>
       </c>
@@ -6223,7 +6308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>67</v>
       </c>
@@ -6237,7 +6322,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>68</v>
       </c>
@@ -6251,7 +6336,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>69</v>
       </c>
@@ -6265,7 +6350,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" ht="41" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>70</v>
       </c>
@@ -6279,7 +6364,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="30" t="s">
         <v>536</v>
       </c>
@@ -6293,7 +6378,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>72</v>
       </c>
@@ -6307,7 +6392,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>74</v>
       </c>
@@ -6321,56 +6406,56 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="34" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="35" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="33"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="33"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" s="29" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B68" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B69" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="21"/>
       <c r="B71" s="28" t="s">
         <v>534</v>
@@ -6378,13 +6463,13 @@
       <c r="C71" s="21"/>
       <c r="D71" s="21"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="21"/>
       <c r="B72" s="16"/>
       <c r="C72" s="21"/>
       <c r="D72" s="21"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="21"/>
       <c r="B73" s="22" t="s">
         <v>100</v>
@@ -6392,7 +6477,7 @@
       <c r="C73" s="21"/>
       <c r="D73" s="21"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="21"/>
       <c r="B74" s="22" t="s">
         <v>101</v>
@@ -6400,12 +6485,12 @@
       <c r="C74" s="21"/>
       <c r="D74" s="21"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B76" s="22" t="s">
         <v>102</v>
       </c>
@@ -6417,21 +6502,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.9140625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -6455,7 +6540,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -6472,7 +6557,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -6489,7 +6574,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -6510,7 +6595,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -6528,7 +6613,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -6549,7 +6634,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -6570,7 +6655,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -6590,7 +6675,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -6610,7 +6695,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -6627,7 +6712,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -6644,7 +6729,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -6661,7 +6746,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -6678,7 +6763,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -6698,7 +6783,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -6718,7 +6803,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -6738,7 +6823,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -6758,7 +6843,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -6778,7 +6863,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -6798,7 +6883,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>118</v>
       </c>
@@ -6818,7 +6903,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -6838,7 +6923,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -6855,7 +6940,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -6872,7 +6957,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -6892,7 +6977,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -6912,7 +6997,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -6932,7 +7017,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -6952,7 +7037,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -6972,7 +7057,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -6992,7 +7077,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -7009,7 +7094,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -7026,7 +7111,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -7043,7 +7128,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -7060,7 +7145,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -7080,7 +7165,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -7100,7 +7185,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -7120,7 +7205,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>120</v>
       </c>
@@ -7140,7 +7225,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>118</v>
       </c>
@@ -7160,7 +7245,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -7180,7 +7265,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -7203,7 +7288,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -7229,21 +7314,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.58203125" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>110</v>
       </c>
@@ -7264,7 +7349,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -7281,7 +7366,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -7298,7 +7383,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -7321,22 +7406,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="13.9140625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
@@ -7355,7 +7440,7 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>129</v>
       </c>
@@ -7374,7 +7459,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -7388,7 +7473,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -7408,23 +7493,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.4140625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
     <col min="4" max="4" width="43.83203125" customWidth="1"/>
-    <col min="5" max="5" width="22.4140625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
@@ -7434,12 +7519,12 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
         <v>158</v>
       </c>
@@ -7448,7 +7533,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -7462,7 +7547,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -7476,12 +7561,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -7495,7 +7580,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -7512,7 +7597,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>194</v>
       </c>
@@ -7536,21 +7621,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
-    <col min="3" max="3" width="39.9140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>109</v>
       </c>
@@ -7569,7 +7654,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -7583,7 +7668,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -7603,23 +7688,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
-    <col min="3" max="3" width="66.4140625" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" customWidth="1"/>
     <col min="5" max="5" width="58.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.4140625" customWidth="1"/>
+    <col min="6" max="6" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>529</v>
       </c>
@@ -7633,27 +7718,27 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="1"/>
       <c r="E2" s="24"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use parameter dataframe indexes to assign disease module parameters
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression.xlsx
+++ b/resources/ResourceFile_Depression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63BAB66-3E18-6B4F-BB8B-D16BEBD132FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1901AE-4573-1144-A1B3-29B15C4D105A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33960" yWindow="-22580" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="-22580" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="572">
   <si>
     <t>Name:</t>
   </si>
@@ -1790,21 +1790,12 @@
   <si>
     <t xml:space="preserve">   </t>
   </si>
-  <si>
-    <t>init_rp_ever_depr_not_current</t>
-  </si>
-  <si>
-    <t>daly_wt_severe_episode_major_depressive_disorder</t>
-  </si>
-  <si>
-    <t>daly_wt_moderate_episode_major_depressive_disorder</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3085,13 +3076,13 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="90.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3099,25 +3090,25 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
@@ -3125,10 +3116,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
@@ -3136,34 +3127,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="95" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3">
       <c r="B14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3">
       <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3">
       <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
@@ -3171,7 +3162,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
@@ -3179,7 +3170,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3">
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
@@ -3187,19 +3178,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3">
       <c r="B20" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
@@ -3207,19 +3198,19 @@
         <v>43346</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3">
       <c r="B26" s="14"/>
       <c r="C26" s="8"/>
     </row>
@@ -3237,14 +3228,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="24" t="s">
         <v>109</v>
       </c>
@@ -3263,7 +3254,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -3284,7 +3275,7 @@
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -3298,7 +3289,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3312,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -3336,10 +3327,10 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
@@ -3348,7 +3339,7 @@
     <col min="5" max="5" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="24" t="s">
         <v>160</v>
       </c>
@@ -3362,13 +3353,13 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="85">
       <c r="A3" s="1"/>
       <c r="C3" s="27" t="s">
         <v>532</v>
@@ -3377,7 +3368,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="C4" t="s">
         <v>186</v>
       </c>
@@ -3388,7 +3379,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>179</v>
       </c>
@@ -3399,7 +3390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>180</v>
       </c>
@@ -3410,7 +3401,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>181</v>
       </c>
@@ -3421,7 +3412,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="C8" t="s">
         <v>182</v>
       </c>
@@ -3432,7 +3423,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="C9" t="s">
         <v>183</v>
       </c>
@@ -3443,7 +3434,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="C10" t="s">
         <v>184</v>
       </c>
@@ -3454,7 +3445,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="C11" t="s">
         <v>185</v>
       </c>
@@ -3465,7 +3456,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>158</v>
       </c>
@@ -3477,7 +3468,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="C15" t="s">
         <v>65</v>
       </c>
@@ -3488,7 +3479,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="C16" t="s">
         <v>66</v>
       </c>
@@ -3499,7 +3490,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="C17" t="s">
         <v>67</v>
       </c>
@@ -3510,7 +3501,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" t="s">
         <v>68</v>
       </c>
@@ -3521,7 +3512,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" t="s">
         <v>69</v>
       </c>
@@ -3532,7 +3523,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" t="s">
         <v>187</v>
       </c>
@@ -3543,7 +3534,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" t="s">
         <v>188</v>
       </c>
@@ -3563,13 +3554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B2:O598"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+    <sheetView topLeftCell="A419" workbookViewId="0">
+      <selection activeCell="C444" sqref="C444"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -3577,68 +3568,68 @@
         <v>527</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11">
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2">
       <c r="B27" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2">
       <c r="B30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2">
       <c r="B32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15">
       <c r="B33" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15">
       <c r="B34" t="s">
         <v>210</v>
       </c>
@@ -3646,2052 +3637,2052 @@
         <v>528</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15">
       <c r="B35" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15">
       <c r="B36" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15">
       <c r="B37" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15">
       <c r="B38" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15">
       <c r="B39" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15">
       <c r="B40" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15">
       <c r="B41" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15">
       <c r="B42" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15">
       <c r="C43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15">
       <c r="C44" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15">
       <c r="B45" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15">
       <c r="C46" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15">
       <c r="B47" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15">
       <c r="B48" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3">
       <c r="B49" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3">
       <c r="B50" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3">
       <c r="B51" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3">
       <c r="B52" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3">
       <c r="B53" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3">
       <c r="B54" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3">
       <c r="B56" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3">
       <c r="B57" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3">
       <c r="B58" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3">
       <c r="B60" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:3">
       <c r="B61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:3">
       <c r="B62" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:3">
       <c r="C63" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:3">
       <c r="C64" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2">
       <c r="B69" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:2">
       <c r="B72" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2">
       <c r="B73" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2">
       <c r="B74" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2">
       <c r="B75" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2">
       <c r="B76" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2">
       <c r="B77" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2">
       <c r="B78" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2">
       <c r="B79" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2">
       <c r="B80" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2">
       <c r="B83" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2">
       <c r="B85" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2">
       <c r="B86" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2">
       <c r="B87" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:2">
       <c r="B88" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:2">
       <c r="B89" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:2">
       <c r="B90" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:2">
       <c r="B91" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:2">
       <c r="B92" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:2">
       <c r="B93" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:2">
       <c r="B94" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:2">
       <c r="B95" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:2">
       <c r="B96" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:2">
       <c r="B97" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:2">
       <c r="B99" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2">
       <c r="B100" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2">
       <c r="B102" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2">
       <c r="B103" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:2">
       <c r="B104" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:2">
       <c r="B105" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2">
       <c r="B106" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:2">
       <c r="B107" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:2">
       <c r="B108" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2">
       <c r="B109" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:2">
       <c r="B110" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2">
       <c r="B111" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:2">
       <c r="B112" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2">
       <c r="B113" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2">
       <c r="B114" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2">
       <c r="B115" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2">
       <c r="B117" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:2">
       <c r="B119" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:2">
       <c r="B121" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:2">
       <c r="B122" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:2">
       <c r="B124" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:2">
       <c r="B126" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:2">
       <c r="B127" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:2">
       <c r="B128" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:2">
       <c r="B129" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2">
       <c r="B130" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2">
       <c r="B131" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2">
       <c r="B132" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2">
       <c r="B133" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2">
       <c r="B135" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2">
       <c r="B136" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2">
       <c r="B137" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2">
       <c r="B138" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2">
       <c r="B139" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2">
       <c r="B140" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2">
       <c r="B141" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:2">
       <c r="B142" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:3">
       <c r="B145" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:3">
       <c r="C146" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:3">
       <c r="C147" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:3">
       <c r="C148" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:3">
       <c r="C149" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:3">
       <c r="C150" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:3">
       <c r="C151" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:3">
       <c r="C152" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:3">
       <c r="C153" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:3">
       <c r="C154" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:3">
       <c r="C155" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:3">
       <c r="C156" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:3">
       <c r="C157" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:3">
       <c r="B158" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2">
       <c r="B162" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:2">
       <c r="B163" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2">
       <c r="B164" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2">
       <c r="B165" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2">
       <c r="B166" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2">
       <c r="B168" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2">
       <c r="B169" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:2">
       <c r="B170" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:2">
       <c r="B172" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:2">
       <c r="B173" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:2">
       <c r="B174" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:2">
       <c r="B176" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:2">
       <c r="B177" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:2">
       <c r="B178" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:2">
       <c r="B180" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:2">
       <c r="B181" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:2">
       <c r="B182" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:2">
       <c r="B183" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:2">
       <c r="B184" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:2">
       <c r="B186" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:2">
       <c r="B187" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:2">
       <c r="B188" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:2">
       <c r="B191" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:2">
       <c r="B192" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:2">
       <c r="B193" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:2">
       <c r="B194" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:2">
       <c r="B195" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:2">
       <c r="B197" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:2">
       <c r="B198" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:2">
       <c r="B199" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:2">
       <c r="B202" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:2">
       <c r="B203" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:2">
       <c r="B205" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:2">
       <c r="B207" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:2">
       <c r="B208" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2">
       <c r="B209" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2">
       <c r="B210" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2">
       <c r="B211" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2">
       <c r="B213" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:2">
       <c r="B215" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:2">
       <c r="B216" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:2">
       <c r="B217" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:2">
       <c r="B218" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:2">
       <c r="B219" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:2">
       <c r="B222" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:2">
       <c r="B223" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:2">
       <c r="B224" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:4">
       <c r="B225" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:4">
       <c r="B226" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:4">
       <c r="B227" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:4">
       <c r="B228" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:4">
       <c r="B229" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:4">
       <c r="B232" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:4">
       <c r="D233" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:4">
       <c r="D234" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:4">
       <c r="D235" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:4">
       <c r="D236" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:4">
       <c r="D237" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:4">
       <c r="D238" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:4">
       <c r="D239" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:4">
       <c r="B240" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:2">
       <c r="B244" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:2">
       <c r="B245" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:2">
       <c r="B246" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:2">
       <c r="B247" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:2">
       <c r="B251" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:2">
       <c r="B252" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:2">
       <c r="B253" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:2">
       <c r="B255" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:2">
       <c r="B256" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:2">
       <c r="B258" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:2">
       <c r="B260" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:2">
       <c r="B261" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:2">
       <c r="B262" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:2">
       <c r="B263" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:2">
       <c r="B265" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:2">
       <c r="B266" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:2">
       <c r="B267" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:2">
       <c r="B269" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:2">
       <c r="B277" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:2">
       <c r="B278" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:2">
       <c r="B279" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:2">
       <c r="B280" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:2">
       <c r="B282" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:2">
       <c r="B284" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:2">
       <c r="B285" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:2">
       <c r="B287" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:2">
       <c r="B288" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:2">
       <c r="B289" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:2">
       <c r="B291" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:2">
       <c r="B292" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:2">
       <c r="B293" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:2">
       <c r="B295" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:2">
       <c r="B296" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:2">
       <c r="B297" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:2">
       <c r="B298" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:2">
       <c r="B299" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:2">
       <c r="B301" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:2">
       <c r="B302" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:2">
       <c r="B303" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:2">
       <c r="B306" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="307" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:2">
       <c r="B307" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="308" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:2">
       <c r="B308" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="309" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:2">
       <c r="B309" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="310" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:2">
       <c r="B310" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="312" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:2">
       <c r="B312" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="313" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:2">
       <c r="B313" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="314" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:2">
       <c r="B314" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:2">
       <c r="B316" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:2">
       <c r="B322" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:2">
       <c r="B324" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:2">
       <c r="B325" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:2">
       <c r="B326" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="328" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:2">
       <c r="B328" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="329" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:2">
       <c r="B329" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="330" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:2">
       <c r="B330" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="332" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:2">
       <c r="B332" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="333" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:2">
       <c r="B333" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="334" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:2">
       <c r="B334" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="336" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:2">
       <c r="B336" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:3">
       <c r="B337" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:3">
       <c r="B338" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:3">
       <c r="B340" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:3">
       <c r="B343" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:3">
       <c r="B345" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:3">
       <c r="C347" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:3">
       <c r="C349" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:3">
       <c r="C350" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:3">
       <c r="C351" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:3">
       <c r="C352" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="353" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:4">
       <c r="C353" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="354" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:4">
       <c r="D354" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="355" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:4">
       <c r="C355" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="357" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:4">
       <c r="C357" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="360" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:4">
       <c r="C360" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="362" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:4">
       <c r="C362" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="365" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:4">
       <c r="C365" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="367" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:4">
       <c r="C367" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="368" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:4">
       <c r="C368" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="369" spans="2:3">
       <c r="C369" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="372" spans="2:3">
       <c r="C372" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="374" spans="2:3">
       <c r="C374" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="375" spans="2:3">
       <c r="C375" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="377" spans="2:3">
       <c r="C377" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="379" spans="2:3">
       <c r="C379" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="381" spans="2:3">
       <c r="B381" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="384" spans="2:3">
       <c r="B384" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="386" spans="2:3">
       <c r="B386" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="387" spans="2:3">
       <c r="B387" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="388" spans="2:3">
       <c r="B388" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="389" spans="2:3">
       <c r="B389" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="393" spans="2:3">
       <c r="B393" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="395" spans="2:3">
       <c r="B395" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="397" spans="2:3">
       <c r="C397" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="398" spans="2:3">
       <c r="C398" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="399" spans="2:3">
       <c r="C399" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="400" spans="2:3">
       <c r="C400" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="401" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:4">
       <c r="C401" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="402" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:4">
       <c r="C402" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="403" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:4">
       <c r="C403" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="404" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:4">
       <c r="C404" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="405" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:4">
       <c r="C405" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="406" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="3:4">
       <c r="C406" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="407" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="3:4">
       <c r="C407" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="408" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="3:4">
       <c r="C408" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="409" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="3:4">
       <c r="D409" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="410" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="3:4">
       <c r="D410" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="411" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="3:4">
       <c r="D411" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="412" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="3:4">
       <c r="D412" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="413" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="3:4">
       <c r="D413" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="414" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="3:4">
       <c r="D414" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="415" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="3:4">
       <c r="D415" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="416" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="3:4">
       <c r="C416" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="418" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="418" spans="2:2">
       <c r="B418" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="421" spans="2:2">
       <c r="B421" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="423" spans="2:2">
       <c r="B423" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="424" spans="2:2">
       <c r="B424" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="425" spans="2:2">
       <c r="B425" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="428" spans="2:2">
       <c r="B428" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="430" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="430" spans="2:2">
       <c r="B430" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="431" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="431" spans="2:2">
       <c r="B431" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="432" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="432" spans="2:2">
       <c r="B432" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="433" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="433" spans="2:3">
       <c r="B433" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="434" spans="2:3">
       <c r="B434" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="435" spans="2:3">
       <c r="B435" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="438" spans="2:3">
       <c r="B438" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="440" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="440" spans="2:3">
       <c r="B440" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="441" spans="2:3">
       <c r="C441" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="442" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="442" spans="2:3">
       <c r="C442" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="443" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="443" spans="2:3">
       <c r="C443" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="444" spans="2:3">
       <c r="C444" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="445" spans="2:3">
       <c r="C445" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="446" spans="2:3">
       <c r="C446" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="447" spans="2:3">
       <c r="B447" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="449" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="449" spans="2:2">
       <c r="B449" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="453" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="453" spans="2:2">
       <c r="B453" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="455" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="455" spans="2:2">
       <c r="B455" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="456" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="456" spans="2:2">
       <c r="B456" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="459" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="459" spans="2:2">
       <c r="B459" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="461" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="461" spans="2:2">
       <c r="B461" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="462" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="462" spans="2:2">
       <c r="B462" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="465" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="465" spans="2:4">
       <c r="B465" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="467" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="467" spans="2:4">
       <c r="B467" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="468" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="468" spans="2:4">
       <c r="B468" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="469" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="469" spans="2:4">
       <c r="B469" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="474" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="474" spans="2:4">
       <c r="B474" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="475" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="475" spans="2:4">
       <c r="C475" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="476" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="476" spans="2:4">
       <c r="D476" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="477" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="477" spans="2:4">
       <c r="D477" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="478" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="478" spans="2:4">
       <c r="D478" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="479" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="479" spans="2:4">
       <c r="D479" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="480" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="480" spans="2:4">
       <c r="D480" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="481" spans="4:4">
       <c r="D481" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="482" spans="4:4">
       <c r="D482" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="483" spans="4:4">
       <c r="D483" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="484" spans="4:4">
       <c r="D484" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="485" spans="4:4">
       <c r="D485" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="486" spans="4:4">
       <c r="D486" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="487" spans="4:4">
       <c r="D487" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="488" spans="4:4">
       <c r="D488" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="489" spans="4:4">
       <c r="D489" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="490" spans="4:4">
       <c r="D490" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="491" spans="4:4">
       <c r="D491" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="492" spans="4:4">
       <c r="D492" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="493" spans="4:4">
       <c r="D493" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="494" spans="4:4">
       <c r="D494" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="495" spans="4:4">
       <c r="D495" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="496" spans="4:4">
       <c r="D496" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="497" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="497" spans="3:4">
       <c r="C497" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="499" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="499" spans="3:4">
       <c r="C499" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="500" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="500" spans="3:4">
       <c r="D500" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="501" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="501" spans="3:4">
       <c r="D501" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="502" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="502" spans="3:4">
       <c r="D502" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="503" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="503" spans="3:4">
       <c r="D503" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="504" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="504" spans="3:4">
       <c r="D504" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="505" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="505" spans="3:4">
       <c r="D505" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="506" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="506" spans="3:4">
       <c r="D506" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="507" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="507" spans="3:4">
       <c r="D507" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="508" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="508" spans="3:4">
       <c r="D508" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="509" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="509" spans="3:4">
       <c r="D509" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="510" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="510" spans="3:4">
       <c r="D510" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="511" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="511" spans="3:4">
       <c r="D511" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="512" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="512" spans="3:4">
       <c r="D512" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="513" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="513" spans="2:4">
       <c r="D513" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="514" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="514" spans="2:4">
       <c r="D514" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="515" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="515" spans="2:4">
       <c r="D515" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="516" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="516" spans="2:4">
       <c r="D516" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="517" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="517" spans="2:4">
       <c r="D517" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="518" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="518" spans="2:4">
       <c r="D518" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="519" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="519" spans="2:4">
       <c r="D519" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="520" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="520" spans="2:4">
       <c r="D520" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="521" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="521" spans="2:4">
       <c r="C521" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="523" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="523" spans="2:4">
       <c r="B523" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="524" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="524" spans="2:4">
       <c r="B524" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="525" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="525" spans="2:4">
       <c r="B525" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="527" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="527" spans="2:4">
       <c r="B527" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="528" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="528" spans="2:4">
       <c r="B528" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="529" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="529" spans="2:2">
       <c r="B529" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="531" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="531" spans="2:2">
       <c r="B531" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="532" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="532" spans="2:2">
       <c r="B532" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="534" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="534" spans="2:2">
       <c r="B534" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="535" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="535" spans="2:2">
       <c r="B535" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="537" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="537" spans="2:2">
       <c r="B537" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="539" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="539" spans="2:2">
       <c r="B539" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="541" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="541" spans="2:2">
       <c r="B541" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="542" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="542" spans="2:2">
       <c r="B542" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="543" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="543" spans="2:2">
       <c r="B543" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="548" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="548" spans="2:2">
       <c r="B548" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="549" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="549" spans="2:2">
       <c r="B549" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="552" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="552" spans="2:2">
       <c r="B552" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="553" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="553" spans="2:2">
       <c r="B553" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="554" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="554" spans="2:2">
       <c r="B554" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="555" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="555" spans="2:2">
       <c r="B555" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="556" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="556" spans="2:2">
       <c r="B556" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="557" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="557" spans="2:2">
       <c r="B557" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="558" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="558" spans="2:2">
       <c r="B558" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="560" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="560" spans="2:2">
       <c r="B560" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="561" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="561" spans="2:2">
       <c r="B561" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="562" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="562" spans="2:2">
       <c r="B562" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="563" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="563" spans="2:2">
       <c r="B563" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="565" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="565" spans="2:2">
       <c r="B565" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="566" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="566" spans="2:2">
       <c r="B566" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="567" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="567" spans="2:2">
       <c r="B567" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="568" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="568" spans="2:2">
       <c r="B568" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="570" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="570" spans="2:2">
       <c r="B570" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="571" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="571" spans="2:2">
       <c r="B571" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="572" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="572" spans="2:2">
       <c r="B572" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="573" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="573" spans="2:2">
       <c r="B573" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="574" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="574" spans="2:2">
       <c r="B574" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="575" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="575" spans="2:2">
       <c r="B575" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="576" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="576" spans="2:2">
       <c r="B576" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="577" spans="2:2">
       <c r="B577" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="579" spans="2:2">
       <c r="B579" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="580" spans="2:2">
       <c r="B580" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="582" spans="2:2">
       <c r="B582" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="583" spans="2:2">
       <c r="B583" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="585" spans="2:2">
       <c r="B585" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="586" spans="2:2">
       <c r="B586" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="587" spans="2:2">
       <c r="B587" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="589" spans="2:2">
       <c r="B589" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="591" spans="2:2">
       <c r="B591" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="592" spans="2:2">
       <c r="B592" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="594" spans="2:2">
       <c r="B594" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="596" spans="2:2">
       <c r="B596" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="598" spans="2:2">
       <c r="B598" t="s">
         <v>488</v>
       </c>
@@ -5704,19 +5695,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>545</v>
       </c>
@@ -5724,7 +5715,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>546</v>
       </c>
@@ -5732,7 +5723,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>547</v>
       </c>
@@ -5740,7 +5731,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>548</v>
       </c>
@@ -5748,7 +5739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>549</v>
       </c>
@@ -5759,7 +5750,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>550</v>
       </c>
@@ -5767,7 +5758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5775,7 +5766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>552</v>
       </c>
@@ -5783,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>553</v>
       </c>
@@ -5791,7 +5782,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>554</v>
       </c>
@@ -5799,7 +5790,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>555</v>
       </c>
@@ -5807,7 +5798,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>556</v>
       </c>
@@ -5815,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>557</v>
       </c>
@@ -5823,7 +5814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>558</v>
       </c>
@@ -5831,7 +5822,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>559</v>
       </c>
@@ -5839,7 +5830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>560</v>
       </c>
@@ -5847,7 +5838,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>561</v>
       </c>
@@ -5858,7 +5849,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>562</v>
       </c>
@@ -5866,7 +5857,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -5874,7 +5865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>563</v>
       </c>
@@ -5882,7 +5873,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>564</v>
       </c>
@@ -5893,7 +5884,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>565</v>
       </c>
@@ -5901,7 +5892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>566</v>
       </c>
@@ -5909,7 +5900,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>567</v>
       </c>
@@ -5917,7 +5908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>568</v>
       </c>
@@ -5925,7 +5916,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -5933,7 +5924,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -5941,7 +5932,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -5949,7 +5940,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>569</v>
       </c>
@@ -5957,7 +5948,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>536</v>
       </c>
@@ -5965,36 +5956,12 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>570</v>
       </c>
       <c r="B31">
         <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>572</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>573</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>574</v>
-      </c>
-      <c r="B34">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6007,11 +5974,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A26:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
@@ -6019,12 +5986,12 @@
     <col min="5" max="5" width="148.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5">
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5">
       <c r="B28" s="1" t="s">
         <v>490</v>
       </c>
@@ -6035,7 +6002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -6046,7 +6013,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -6054,7 +6021,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -6065,7 +6032,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
         <v>32</v>
       </c>
@@ -6076,7 +6043,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -6084,7 +6051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
         <v>53</v>
       </c>
@@ -6098,7 +6065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5">
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -6112,7 +6079,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5">
       <c r="B37" t="s">
         <v>38</v>
       </c>
@@ -6126,7 +6093,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5">
       <c r="B38" t="s">
         <v>40</v>
       </c>
@@ -6140,7 +6107,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -6154,7 +6121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5">
       <c r="B40" t="s">
         <v>44</v>
       </c>
@@ -6168,7 +6135,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5">
       <c r="B41" t="s">
         <v>46</v>
       </c>
@@ -6182,7 +6149,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5">
       <c r="B42" t="s">
         <v>48</v>
       </c>
@@ -6196,7 +6163,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5">
       <c r="B43" t="s">
         <v>50</v>
       </c>
@@ -6210,7 +6177,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5">
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -6224,7 +6191,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5">
       <c r="B45" t="s">
         <v>57</v>
       </c>
@@ -6238,7 +6205,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5">
       <c r="B46" t="s">
         <v>59</v>
       </c>
@@ -6252,7 +6219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5">
       <c r="B47" t="s">
         <v>61</v>
       </c>
@@ -6266,7 +6233,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5">
       <c r="B48" t="s">
         <v>63</v>
       </c>
@@ -6280,7 +6247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5">
       <c r="B49" t="s">
         <v>65</v>
       </c>
@@ -6294,7 +6261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5">
       <c r="B50" t="s">
         <v>66</v>
       </c>
@@ -6308,7 +6275,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5">
       <c r="B51" t="s">
         <v>67</v>
       </c>
@@ -6322,7 +6289,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:5">
       <c r="B52" t="s">
         <v>68</v>
       </c>
@@ -6336,7 +6303,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:5">
       <c r="B53" t="s">
         <v>69</v>
       </c>
@@ -6350,7 +6317,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="41" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5" ht="41">
       <c r="B54" t="s">
         <v>70</v>
       </c>
@@ -6364,7 +6331,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5">
       <c r="B55" s="30" t="s">
         <v>536</v>
       </c>
@@ -6378,7 +6345,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5">
       <c r="B56" t="s">
         <v>72</v>
       </c>
@@ -6392,7 +6359,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5">
       <c r="B57" t="s">
         <v>74</v>
       </c>
@@ -6406,56 +6373,56 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5">
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5" s="25" customFormat="1">
       <c r="B59" s="34" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="60" spans="2:5" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5" s="25" customFormat="1">
       <c r="B60" s="35" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:5">
       <c r="B61" s="33"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5">
       <c r="B62" s="33"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:5">
       <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="B65" s="29" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="17">
       <c r="B66" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="B67" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="B68" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="B69" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="21"/>
       <c r="B71" s="28" t="s">
         <v>534</v>
@@ -6463,13 +6430,13 @@
       <c r="C71" s="21"/>
       <c r="D71" s="21"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="21"/>
       <c r="B72" s="16"/>
       <c r="C72" s="21"/>
       <c r="D72" s="21"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="21"/>
       <c r="B73" s="22" t="s">
         <v>100</v>
@@ -6477,7 +6444,7 @@
       <c r="C73" s="21"/>
       <c r="D73" s="21"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="21"/>
       <c r="B74" s="22" t="s">
         <v>101</v>
@@ -6485,12 +6452,12 @@
       <c r="C74" s="21"/>
       <c r="D74" s="21"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="B75" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="B76" s="22" t="s">
         <v>102</v>
       </c>
@@ -6509,14 +6476,14 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -6540,7 +6507,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>117</v>
       </c>
@@ -6557,7 +6524,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -6574,7 +6541,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -6595,7 +6562,7 @@
       </c>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -6613,7 +6580,7 @@
       </c>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -6634,7 +6601,7 @@
       </c>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -6655,7 +6622,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -6675,7 +6642,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -6695,7 +6662,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -6712,7 +6679,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -6729,7 +6696,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -6746,7 +6713,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -6763,7 +6730,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -6783,7 +6750,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -6803,7 +6770,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -6823,7 +6790,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -6843,7 +6810,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -6863,7 +6830,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -6883,7 +6850,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>118</v>
       </c>
@@ -6903,7 +6870,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -6923,7 +6890,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -6940,7 +6907,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -6957,7 +6924,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -6977,7 +6944,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -6997,7 +6964,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -7017,7 +6984,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -7037,7 +7004,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -7057,7 +7024,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -7077,7 +7044,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -7094,7 +7061,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -7111,7 +7078,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>119</v>
       </c>
@@ -7128,7 +7095,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -7145,7 +7112,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -7165,7 +7132,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -7185,7 +7152,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -7205,7 +7172,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>120</v>
       </c>
@@ -7225,7 +7192,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>118</v>
       </c>
@@ -7245,7 +7212,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -7265,7 +7232,7 @@
         <v>0.60750000000000004</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -7288,7 +7255,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -7321,14 +7288,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="23" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>110</v>
       </c>
@@ -7349,7 +7316,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -7366,7 +7333,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -7383,7 +7350,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -7413,7 +7380,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
@@ -7421,7 +7388,7 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="24" t="s">
         <v>13</v>
       </c>
@@ -7440,7 +7407,7 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="23" t="s">
         <v>129</v>
       </c>
@@ -7459,7 +7426,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -7473,7 +7440,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -7500,7 +7467,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
@@ -7509,7 +7476,7 @@
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
@@ -7519,12 +7486,12 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="B3" s="24" t="s">
         <v>158</v>
       </c>
@@ -7533,7 +7500,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -7547,7 +7514,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -7561,12 +7528,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="D8" s="24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -7580,7 +7547,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -7597,7 +7564,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>194</v>
       </c>
@@ -7628,14 +7595,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="24" t="s">
         <v>109</v>
       </c>
@@ -7654,7 +7621,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>192</v>
       </c>
@@ -7668,7 +7635,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -7695,7 +7662,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="66.33203125" customWidth="1"/>
@@ -7704,7 +7671,7 @@
     <col min="6" max="6" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="24" t="s">
         <v>529</v>
       </c>
@@ -7718,27 +7685,27 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="1"/>
       <c r="E2" s="24"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="25"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overall structure of HSI ready for testing
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression.xlsx
+++ b/resources/ResourceFile_Depression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbh03/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC6A60-15C5-F34E-8ED9-7D5949146832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F529BE8-D182-E946-9F5D-3B9A436765C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27240" windowHeight="18800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="590">
   <si>
     <t>Name:</t>
   </si>
@@ -1838,12 +1838,18 @@
   <si>
     <t>specificity_of_assessment_of_depression</t>
   </si>
+  <si>
+    <t>pr_assessed_for_depression_in_generic_appt_level1</t>
+  </si>
+  <si>
+    <t>anti_depressant_medication_item_code</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1963,8 +1969,14 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1974,6 +1986,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2078,7 +2096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2162,6 +2180,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6748,10 +6769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A37"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6987,7 +7008,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="43" t="s">
         <v>52</v>
       </c>
       <c r="B28">
@@ -6995,7 +7016,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="42" t="s">
         <v>55</v>
       </c>
       <c r="B29">
@@ -7003,7 +7024,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="42" t="s">
         <v>53</v>
       </c>
       <c r="B30">
@@ -7064,6 +7085,22 @@
       </c>
       <c r="B37" s="40">
         <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="s">
+        <v>588</v>
+      </c>
+      <c r="B38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="39" t="s">
+        <v>589</v>
+      </c>
+      <c r="B39" s="41">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests on the properties configurations complete
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression.xlsx
+++ b/resources/ResourceFile_Depression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbh03/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F529BE8-D182-E946-9F5D-3B9A436765C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140152A2-DE89-DF4D-BF3E-226D6CF9D12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27240" windowHeight="18800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,17 +26,25 @@
     <sheet name="pr change in depression status_" sheetId="13" r:id="rId11"/>
     <sheet name="References" sheetId="7" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="589">
   <si>
     <t>Name:</t>
   </si>
@@ -1834,9 +1842,6 @@
   </si>
   <si>
     <t>sensitivity_of_assessment_of_depression</t>
-  </si>
-  <si>
-    <t>specificity_of_assessment_of_depression</t>
   </si>
   <si>
     <t>pr_assessed_for_depression_in_generic_appt_level1</t>
@@ -2096,7 +2101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2179,7 +2184,6 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -6769,10 +6773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7008,7 +7012,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B28">
@@ -7016,7 +7020,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="41" t="s">
         <v>55</v>
       </c>
       <c r="B29">
@@ -7024,7 +7028,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="41" t="s">
         <v>53</v>
       </c>
       <c r="B30">
@@ -7083,23 +7087,15 @@
       <c r="A37" s="39" t="s">
         <v>587</v>
       </c>
-      <c r="B37" s="40">
-        <v>1</v>
+      <c r="B37">
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="39" t="s">
         <v>588</v>
       </c>
-      <c r="B38">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="39" t="s">
-        <v>589</v>
-      </c>
-      <c r="B39" s="41">
+      <c r="B38" s="40">
         <v>267</v>
       </c>
     </row>
@@ -7113,7 +7109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A26:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replace depression resourcefile with update
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Depression.xlsx
+++ b/resources/ResourceFile_Depression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbh03/PycharmProjects/TLOmodel/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Dropbox\Thanzi la Onse\04 - Methods Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD8A6C-9B68-8941-9166-86948ACE048E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398D85DE-FFF7-454C-BA27-09EC1CBF6547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40100" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="14" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>rr_depr_prev_epis</t>
   </si>
@@ -189,6 +181,18 @@
   </si>
   <si>
     <t>prob_3m_default_antidepr</t>
+  </si>
+  <si>
+    <t>init_pr_ever_talking_therapy_if_diagnosed</t>
+  </si>
+  <si>
+    <t>We assume that talking therapy happens as part of diagnosis</t>
+  </si>
+  <si>
+    <t>init_pr_ever_self_harmed_if_ever_depr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consistent with rate of incident self harm </t>
   </si>
 </sst>
 </file>
@@ -632,13 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -647,7 +651,7 @@
     <col min="5" max="5" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -658,7 +662,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -669,7 +673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -680,7 +684,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -691,7 +695,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -705,7 +709,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -716,7 +720,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -727,7 +731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -738,7 +742,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -749,7 +753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -760,7 +764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -771,7 +775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -782,7 +786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -793,231 +797,253 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B16" s="5">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="B17" s="5">
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="5">
         <v>3</v>
       </c>
-      <c r="H17" t="s">
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B20" s="5">
         <v>1.5</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B21" s="5">
         <v>50</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B22" s="5">
         <v>30</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B23" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B24" s="5">
         <v>3</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B26" s="5">
         <v>0.5</v>
       </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B27" s="5">
         <v>1.5</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B28" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B29" s="5">
         <v>0.7</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B30" s="5">
         <v>0.2</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="D30" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B31" s="5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B32" s="5">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B33" s="11">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="D33" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B34" s="5">
         <v>0.75</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="D34" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B35" s="5">
         <v>0.5</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B36" s="5">
         <v>267</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>